<commit_message>
working import for excel file
</commit_message>
<xml_diff>
--- a/Ride Group Template.xlsx
+++ b/Ride Group Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/568bd6e1322fdf29/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Lee\Documents\GitHub\JSA-Ride-Groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2826B073-C60D-48E5-B278-21E3819378BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F74F0CF-7DEB-40DC-AE0E-2A98EABB2CF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3F4AF8C-E471-4BDE-958A-C2B9B05D0B65}"/>
   </bookViews>
@@ -28,6 +28,122 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Providing Rides?</t>
+  </si>
+  <si>
+    <t>Car Size (including driver)</t>
+  </si>
+  <si>
+    <t>Drop Off</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ERC</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>La Regencia</t>
+  </si>
+  <si>
+    <t>I-House</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Solazzo</t>
+  </si>
+  <si>
+    <t>Costa Verde</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>Person A</t>
+  </si>
+  <si>
+    <t>Person B</t>
+  </si>
+  <si>
+    <t>Person C</t>
+  </si>
+  <si>
+    <t>Person D</t>
+  </si>
+  <si>
+    <t>Person E</t>
+  </si>
+  <si>
+    <t>Person F</t>
+  </si>
+  <si>
+    <t>Person G</t>
+  </si>
+  <si>
+    <t>Person H</t>
+  </si>
+  <si>
+    <t>Person I</t>
+  </si>
+  <si>
+    <t>Person J</t>
+  </si>
+  <si>
+    <t>Person K</t>
+  </si>
+  <si>
+    <t>Person L</t>
+  </si>
+  <si>
+    <t>Person M</t>
+  </si>
+  <si>
+    <t>Person N</t>
+  </si>
+  <si>
+    <t>Person O</t>
+  </si>
+  <si>
+    <t>Person P</t>
+  </si>
+  <si>
+    <t>Person Q</t>
+  </si>
+  <si>
+    <t>Person R</t>
+  </si>
+  <si>
+    <t>Person S</t>
+  </si>
+  <si>
+    <t>Person T</t>
+  </si>
+  <si>
+    <t>Vons</t>
+  </si>
+  <si>
+    <t>Pines of La Jolla</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,8 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +496,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BFD76E-D6AC-4CE6-9C49-F3EFDF314D87}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>